<commit_message>
Add run time, pace and speed in Laufdaten.xlsx.
</commit_message>
<xml_diff>
--- a/Laufdaten.xlsx
+++ b/Laufdaten.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Malte Fritz\Documents\git\run_with_fun\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DC03D6-CACA-461E-90C9-8DB02FCB9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730"/>
+    <workbookView xWindow="57480" yWindow="16185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -35,11 +46,20 @@
   <si>
     <t>sec</t>
   </si>
+  <si>
+    <t>run time</t>
+  </si>
+  <si>
+    <t>pace</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -840,16 +860,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -865,8 +885,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44756</v>
       </c>
@@ -880,23 +909,47 @@
         <v>30</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <f>(C2*60)+D2+(E2/60)</f>
+        <v>30.833333333333332</v>
+      </c>
+      <c r="H2">
+        <f>G2/B2</f>
+        <v>5.1388888888888884</v>
+      </c>
+      <c r="I2">
+        <f>B2/(G2/60)</f>
+        <v>11.675675675675677</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44758</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D3">
-        <v>29</v>
-      </c>
       <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>(C3*60)+D3+(E3/60)</f>
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <f>G3/B3</f>
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <f>B3/(G3/60)</f>
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add a test run.
</commit_message>
<xml_diff>
--- a/Laufdaten.xlsx
+++ b/Laufdaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Malte Fritz\Documents\git\run_with_fun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DC03D6-CACA-461E-90C9-8DB02FCB9D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7E627-AFCF-4E28-AB07-CEBFCE0FC171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="16185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3015" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -537,9 +537,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -861,16 +863,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="7" max="9" width="11.42578125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -885,17 +891,17 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44756</v>
       </c>
@@ -911,20 +917,20 @@
       <c r="E2">
         <v>50</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <f>(C2*60)+D2+(E2/60)</f>
         <v>30.833333333333332</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <f>G2/B2</f>
         <v>5.1388888888888884</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <f>B2/(G2/60)</f>
         <v>11.675675675675677</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44758</v>
       </c>
@@ -940,20 +946,50 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <f>(C3*60)+D3+(E3/60)</f>
         <v>60</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <f>G3/B3</f>
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <f>B3/(G3/60)</f>
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44761</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <f>(C4*60)+D4+(E4/60)</f>
+        <v>12.05</v>
+      </c>
+      <c r="H4" s="2">
+        <f>G4/B4</f>
+        <v>6.0250000000000004</v>
+      </c>
+      <c r="I4" s="2">
+        <f>B4/(G4/60)</f>
+        <v>9.9585062240663902</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add some running examples.
</commit_message>
<xml_diff>
--- a/Laufdaten.xlsx
+++ b/Laufdaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Malte Fritz\Documents\git\run_with_fun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7E627-AFCF-4E28-AB07-CEBFCE0FC171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F12446C-EF87-4DD4-9566-483F8FB6567A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3015" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,6 +988,151 @@
         <v>9.9585062240663902</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44766</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="G5" s="2">
+        <f>(C5*60)+D5+(E5/60)</f>
+        <v>11.75</v>
+      </c>
+      <c r="H5" s="2">
+        <f>G5/B5</f>
+        <v>3.9166666666666665</v>
+      </c>
+      <c r="I5" s="2">
+        <f>B5/(G5/60)</f>
+        <v>15.319148936170214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44767</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2">
+        <f>(C6*60)+D6+(E6/60)</f>
+        <v>6.25</v>
+      </c>
+      <c r="H6" s="2">
+        <f>G6/B6</f>
+        <v>3.125</v>
+      </c>
+      <c r="I6" s="2">
+        <f>B6/(G6/60)</f>
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44769</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <f>(C7*60)+D7+(E7/60)</f>
+        <v>30</v>
+      </c>
+      <c r="H7" s="2">
+        <f>G7/B7</f>
+        <v>6</v>
+      </c>
+      <c r="I7" s="2">
+        <f>B7/(G7/60)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44770</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>55</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <f>(C8*60)+D8+(E8/60)</f>
+        <v>55</v>
+      </c>
+      <c r="H8" s="2">
+        <f>G8/B8</f>
+        <v>5.5</v>
+      </c>
+      <c r="I8" s="2">
+        <f>B8/(G8/60)</f>
+        <v>10.90909090909091</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44772</v>
+      </c>
+      <c r="B9">
+        <v>21.0975</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>35</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f>(C9*60)+D9+(E9/60)</f>
+        <v>95</v>
+      </c>
+      <c r="H9" s="2">
+        <f>G9/B9</f>
+        <v>4.5029031875814667</v>
+      </c>
+      <c r="I9" s="2">
+        <f>B9/(G9/60)</f>
+        <v>13.324736842105263</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>